<commit_message>
Uploading new Artelys and Agora files
</commit_message>
<xml_diff>
--- a/InputData/trans/BPP/Battery Pack Price.xlsx
+++ b/InputData/trans/BPP/Battery Pack Price.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabian.hein\Desktop\EPS_new\transport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48359E06-F382-4E1F-81F2-5E8970E7301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{AA50C181-653E-490C-BC0D-5D52AA04505F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E181D6E7-0417-4E10-BBDB-256B29017155}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="BPP" sheetId="2" r:id="rId2"/>
-    <sheet name="SYBPP" sheetId="3" r:id="rId3"/>
+    <sheet name="Calculations" sheetId="4" r:id="rId2"/>
+    <sheet name="BPP" sheetId="2" r:id="rId3"/>
+    <sheet name="SYBPP" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -35,30 +39,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>BPP Battery Pack Price</t>
+  </si>
   <si>
     <t>Sources:</t>
   </si>
   <si>
-    <t>BNEF</t>
-  </si>
-  <si>
-    <t>https://about.bnef.com/blog/lithium-ion-battery-pack-prices-rise-for-first-time-to-an-average-of-151-kwh/</t>
-  </si>
-  <si>
-    <t>Lithium-ion Battery Pack Prices Rise for First Time to an Average of $151/kWh</t>
-  </si>
-  <si>
-    <t>2012 to 2022 USD</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>$/kWh</t>
-  </si>
-  <si>
-    <t>BPP Battery Pack Price</t>
+    <r>
+      <t xml:space="preserve">Agora Verkehrswende (2024): </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not yet published</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, working title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Costs of the transport transition</t>
+    </r>
   </si>
   <si>
     <t>Notes:</t>
@@ -67,20 +89,33 @@
     <t>The EPS applies endogenous learning for battery pack prices in years where the battery pack price is listed as 0.</t>
   </si>
   <si>
-    <t>2022 to 2023</t>
+    <t>€ 2023 to $ 2023</t>
   </si>
   <si>
-    <t>Lithium-ion Battery Pack Prices Hit Record Low of $139/kWh</t>
+    <t>$ 2023 to $ 2012</t>
   </si>
   <si>
-    <t>https://about.bnef.com/blog/lithium-ion-battery-pack-prices-hit-record-low-of-139-kwh/#:~:text=Given%20this%2C%20BNEF%20expects%20average,and%20%2480%2FkWh%20in%202030.</t>
+    <t>year</t>
+  </si>
+  <si>
+    <t>2023 € /kWh</t>
+  </si>
+  <si>
+    <t>$/kWh</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +131,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,18 +170,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,90 +510,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF982137-6F01-4109-8226-D4C6F3731BA9}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="101.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.29</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>1/0.951</f>
-        <v>1.0515247108307046</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6">
+        <v>1.083711667</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6">
+        <v>0.754</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -529,247 +575,782 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B959006-9959-4256-ABC6-A7FF52908FE1}">
+  <dimension ref="A2:AG3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2+1</f>
+        <v>2020</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:AF2" si="0">C2+1</f>
+        <v>2021</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="H2" s="3">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="K2" s="3">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="L2" s="3">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="M2" s="3">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="N2" s="3">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="P2" s="3">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="Q2" s="3">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="R2" s="3">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="S2" s="3">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="T2" s="3">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="U2" s="3">
+        <f>T2+1</f>
+        <v>2038</v>
+      </c>
+      <c r="V2" s="3">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="W2" s="3">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="X2" s="3">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="Y2" s="3">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="Z2" s="3">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="AA2" s="3">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="AB2" s="3">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="AC2" s="3">
+        <f>AB2+1</f>
+        <v>2046</v>
+      </c>
+      <c r="AD2" s="3">
+        <f>AC2+1</f>
+        <v>2047</v>
+      </c>
+      <c r="AE2" s="3">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="AF2" s="3">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="AG2" s="3">
+        <f>AF2+1</f>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>163.39285714285714</v>
+      </c>
+      <c r="C3" s="4">
+        <v>140.35087719298247</v>
+      </c>
+      <c r="D3" s="4">
+        <v>127.11864406779662</v>
+      </c>
+      <c r="E3" s="4">
+        <v>153.33333333333331</v>
+      </c>
+      <c r="F3" s="4">
+        <v>128.7037037037037</v>
+      </c>
+      <c r="G3" s="4">
+        <v>123.14814814814814</v>
+      </c>
+      <c r="H3" s="4">
+        <v>104.62962962962962</v>
+      </c>
+      <c r="I3" s="4">
+        <v>98.518518518518519</v>
+      </c>
+      <c r="J3" s="4">
+        <v>92.407407407407405</v>
+      </c>
+      <c r="K3" s="4">
+        <v>86.296296296296305</v>
+      </c>
+      <c r="L3" s="4">
+        <v>80.185185185185205</v>
+      </c>
+      <c r="M3" s="4">
+        <v>74.074074074074076</v>
+      </c>
+      <c r="N3" s="4">
+        <v>71.481481481481481</v>
+      </c>
+      <c r="O3" s="4">
+        <v>68.979629629629628</v>
+      </c>
+      <c r="P3" s="4">
+        <v>66.565342592592586</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>64.235555601851843</v>
+      </c>
+      <c r="R3" s="4">
+        <v>61.987311155787026</v>
+      </c>
+      <c r="S3" s="4">
+        <v>59.817755265334476</v>
+      </c>
+      <c r="T3" s="4">
+        <v>57.724133831047766</v>
+      </c>
+      <c r="U3" s="4">
+        <v>55.703789146961093</v>
+      </c>
+      <c r="V3" s="4">
+        <v>53.754156526817454</v>
+      </c>
+      <c r="W3" s="4">
+        <v>51.872761048378841</v>
+      </c>
+      <c r="X3" s="4">
+        <v>51.354033437895055</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>50.840493103516103</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>50.332088172480944</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>49.828767290756133</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>49.330479617848574</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>48.837174821670089</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>48.348803073453389</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>47.865315042718855</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>47.386661892291663</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>46.912795273368744</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB58F1CD-3AD5-4A1E-8AA0-C74AF29D4BF2}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E1">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F1">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G1">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="H1">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="I1">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="J1">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="K1">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="L1">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="M1">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="N1">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="O1">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="P1">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="Q1">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="R1">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="S1">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="T1">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="U1">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="V1">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="W1">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="X1">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="Y1">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="Z1">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AA1">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AB1">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AC1">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AD1">
-        <v>2049</v>
-      </c>
-      <c r="AE1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <f>141/About!$A$16</f>
-        <v>109.30232558139535</v>
-      </c>
-      <c r="C2">
-        <f>151/About!$A$16</f>
-        <v>117.05426356589147</v>
-      </c>
-      <c r="D2">
-        <f>139/(About!A16*About!A17)</f>
-        <v>102.47209302325579</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B2" s="7">
+        <f>Calculations!E3*About!$A$13*About!$A$14</f>
+        <v>125.29151819409331</v>
+      </c>
+      <c r="C2" s="7">
+        <f>Calculations!F3*About!$A$13*About!$A$14</f>
+        <v>105.16618978852036</v>
+      </c>
+      <c r="D2" s="7">
+        <f>Calculations!G3*About!$A$13*About!$A$14</f>
+        <v>100.62664202786479</v>
+      </c>
+      <c r="E2" s="7">
+        <f>Calculations!H3*About!$A$13*About!$A$14</f>
+        <v>85.494816159012956</v>
+      </c>
+      <c r="F2" s="7">
+        <f>Calculations!I3*About!$A$13*About!$A$14</f>
+        <v>80.501313622291846</v>
+      </c>
+      <c r="G2" s="7">
+        <f>Calculations!J3*About!$A$13*About!$A$14</f>
+        <v>75.507811085570737</v>
+      </c>
+      <c r="H2" s="7">
+        <f>Calculations!K3*About!$A$13*About!$A$14</f>
+        <v>70.514308548849641</v>
+      </c>
+      <c r="I2" s="7">
+        <f>Calculations!L3*About!$A$13*About!$A$14</f>
+        <v>65.520806012128531</v>
+      </c>
+      <c r="J2" s="7">
+        <f>Calculations!M3*About!$A$13*About!$A$14</f>
+        <v>60.527303475407408</v>
+      </c>
+      <c r="K2" s="7">
+        <f>Calculations!N3*About!$A$13*About!$A$14</f>
+        <v>58.408847853768144</v>
+      </c>
+      <c r="L2" s="7">
+        <f>Calculations!O3*About!$A$13*About!$A$14</f>
+        <v>56.364538178886257</v>
+      </c>
+      <c r="M2" s="7">
+        <f>Calculations!P3*About!$A$13*About!$A$14</f>
+        <v>54.391779342625242</v>
+      </c>
+      <c r="N2" s="7">
+        <f>Calculations!Q3*About!$A$13*About!$A$14</f>
+        <v>52.488067065633352</v>
+      </c>
+      <c r="O2" s="7">
+        <f>Calculations!R3*About!$A$13*About!$A$14</f>
+        <v>50.650984718336183</v>
+      </c>
+      <c r="P2" s="7">
+        <f>Calculations!S3*About!$A$13*About!$A$14</f>
+        <v>48.878200253194407</v>
+      </c>
+      <c r="Q2" s="7">
+        <f>Calculations!T3*About!$A$13*About!$A$14</f>
+        <v>47.167463244332609</v>
+      </c>
+      <c r="R2" s="7">
+        <f>Calculations!U3*About!$A$13*About!$A$14</f>
+        <v>45.516602030780966</v>
+      </c>
+      <c r="S2" s="7">
+        <f>Calculations!V3*About!$A$13*About!$A$14</f>
+        <v>43.92352095970363</v>
+      </c>
+      <c r="T2" s="7">
+        <f>Calculations!W3*About!$A$13*About!$A$14</f>
+        <v>42.386197726113998</v>
+      </c>
+      <c r="U2" s="7">
+        <f>Calculations!X3*About!$A$13*About!$A$14</f>
+        <v>41.962335748852865</v>
+      </c>
+      <c r="V2" s="7">
+        <f>Calculations!Y3*About!$A$13*About!$A$14</f>
+        <v>41.542712391364333</v>
+      </c>
+      <c r="W2" s="7">
+        <f>Calculations!Z3*About!$A$13*About!$A$14</f>
+        <v>41.127285267450688</v>
+      </c>
+      <c r="X2" s="7">
+        <f>Calculations!AA3*About!$A$13*About!$A$14</f>
+        <v>40.716012414776188</v>
+      </c>
+      <c r="Y2" s="7">
+        <f>Calculations!AB3*About!$A$13*About!$A$14</f>
+        <v>40.308852290628423</v>
+      </c>
+      <c r="Z2" s="7">
+        <f>Calculations!AC3*About!$A$13*About!$A$14</f>
+        <v>39.905763767722142</v>
+      </c>
+      <c r="AA2" s="7">
+        <f>Calculations!AD3*About!$A$13*About!$A$14</f>
+        <v>39.506706130044918</v>
+      </c>
+      <c r="AB2" s="7">
+        <f>Calculations!AE3*About!$A$13*About!$A$14</f>
+        <v>39.111639068744466</v>
+      </c>
+      <c r="AC2" s="7">
+        <f>Calculations!AF3*About!$A$13*About!$A$14</f>
+        <v>38.720522678057023</v>
+      </c>
+      <c r="AD2" s="7">
+        <f>Calculations!AG3*About!$A$13*About!$A$14</f>
+        <v>38.33331745127645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="B3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC3C966-6AEE-455B-8285-F6B514229E67}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <f>150/About!$A$16</f>
-        <v>116.27906976744185</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <f>Calculations!D3*About!A13*About!A14</f>
+        <v>103.87100808279662</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42629057-6501-4BCD-ADDE-2769C765847E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F07FEF0-D9CD-4745-AA90-3B402C6D0735}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AF123D-D771-4054-8238-EEAACFB07BC7}"/>
 </file>
</xml_diff>

<commit_message>
Calculate transportation battery pack prices endogenously after 2023
</commit_message>
<xml_diff>
--- a/InputData/trans/BPP/Battery Pack Price.xlsx
+++ b/InputData/trans/BPP/Battery Pack Price.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\BPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\BPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F86AFF3-5CDE-4CA8-ABC7-45BABD382112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10696FE-9197-40DC-801B-C06036559853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="3150" windowWidth="19245" windowHeight="11595" activeTab="2" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
+    <workbookView xWindow="2565" yWindow="720" windowWidth="25155" windowHeight="14790" activeTab="2" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>BPP Battery Pack Price</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t>Price</t>
   </si>
+  <si>
+    <t>Use endogenous learning in EPS for future years</t>
+  </si>
 </sst>
 </file>
 
@@ -154,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -196,7 +205,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -216,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,17 +527,17 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="101.28515625" customWidth="1"/>
+    <col min="2" max="2" width="101.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -536,26 +545,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1.083711667</v>
       </c>
@@ -563,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>0.754</v>
       </c>
@@ -578,15 +587,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B959006-9959-4256-ABC6-A7FF52908FE1}">
-  <dimension ref="A2:AG3"/>
+  <dimension ref="A2:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -718,7 +727,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -817,6 +826,94 @@
       </c>
       <c r="AG3" s="4">
         <v>46.912795273368744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9">
+        <v>0</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0</v>
+      </c>
+      <c r="T4" s="9">
+        <v>0</v>
+      </c>
+      <c r="U4" s="9">
+        <v>0</v>
+      </c>
+      <c r="V4" s="9">
+        <v>0</v>
+      </c>
+      <c r="W4" s="9">
+        <v>0</v>
+      </c>
+      <c r="X4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="G6" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -832,16 +929,15 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="9"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -936,7 +1032,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -953,116 +1049,115 @@
         <v>105.16618978852036</v>
       </c>
       <c r="E2" s="8">
-        <f>Calculations!G3*About!$A$13*About!$A$14</f>
-        <v>100.62664202786479</v>
+        <f>Calculations!G4</f>
+        <v>0</v>
       </c>
       <c r="F2" s="8">
-        <f>Calculations!H3*About!$A$13*About!$A$14</f>
-        <v>85.494816159012956</v>
+        <f>Calculations!H4</f>
+        <v>0</v>
       </c>
       <c r="G2" s="8">
-        <f>Calculations!I3*About!$A$13*About!$A$14</f>
-        <v>80.501313622291846</v>
+        <f>Calculations!I4</f>
+        <v>0</v>
       </c>
       <c r="H2" s="8">
-        <f>Calculations!J3*About!$A$13*About!$A$14</f>
-        <v>75.507811085570737</v>
+        <f>Calculations!J4</f>
+        <v>0</v>
       </c>
       <c r="I2" s="8">
-        <f>Calculations!K3*About!$A$13*About!$A$14</f>
-        <v>70.514308548849641</v>
+        <f>Calculations!K4</f>
+        <v>0</v>
       </c>
       <c r="J2" s="8">
-        <f>Calculations!L3*About!$A$13*About!$A$14</f>
-        <v>65.520806012128531</v>
+        <f>Calculations!L4</f>
+        <v>0</v>
       </c>
       <c r="K2" s="8">
-        <f>Calculations!M3*About!$A$13*About!$A$14</f>
-        <v>60.527303475407408</v>
+        <f>Calculations!M4</f>
+        <v>0</v>
       </c>
       <c r="L2" s="8">
-        <f>Calculations!N3*About!$A$13*About!$A$14</f>
-        <v>58.408847853768144</v>
+        <f>Calculations!N4</f>
+        <v>0</v>
       </c>
       <c r="M2" s="8">
-        <f>Calculations!O3*About!$A$13*About!$A$14</f>
-        <v>56.364538178886257</v>
+        <f>Calculations!O4</f>
+        <v>0</v>
       </c>
       <c r="N2" s="8">
-        <f>Calculations!P3*About!$A$13*About!$A$14</f>
-        <v>54.391779342625242</v>
+        <f>Calculations!P4</f>
+        <v>0</v>
       </c>
       <c r="O2" s="8">
-        <f>Calculations!Q3*About!$A$13*About!$A$14</f>
-        <v>52.488067065633352</v>
+        <f>Calculations!Q4</f>
+        <v>0</v>
       </c>
       <c r="P2" s="8">
-        <f>Calculations!R3*About!$A$13*About!$A$14</f>
-        <v>50.650984718336183</v>
+        <f>Calculations!R4</f>
+        <v>0</v>
       </c>
       <c r="Q2" s="8">
-        <f>Calculations!S3*About!$A$13*About!$A$14</f>
-        <v>48.878200253194407</v>
+        <f>Calculations!S4</f>
+        <v>0</v>
       </c>
       <c r="R2" s="8">
-        <f>Calculations!T3*About!$A$13*About!$A$14</f>
-        <v>47.167463244332609</v>
+        <f>Calculations!T4</f>
+        <v>0</v>
       </c>
       <c r="S2" s="8">
-        <f>Calculations!U3*About!$A$13*About!$A$14</f>
-        <v>45.516602030780966</v>
+        <f>Calculations!U4</f>
+        <v>0</v>
       </c>
       <c r="T2" s="8">
-        <f>Calculations!V3*About!$A$13*About!$A$14</f>
-        <v>43.92352095970363</v>
+        <f>Calculations!V4</f>
+        <v>0</v>
       </c>
       <c r="U2" s="8">
-        <f>Calculations!W3*About!$A$13*About!$A$14</f>
-        <v>42.386197726113998</v>
+        <f>Calculations!W4</f>
+        <v>0</v>
       </c>
       <c r="V2" s="8">
-        <f>Calculations!X3*About!$A$13*About!$A$14</f>
-        <v>41.962335748852865</v>
+        <f>Calculations!X4</f>
+        <v>0</v>
       </c>
       <c r="W2" s="8">
-        <f>Calculations!Y3*About!$A$13*About!$A$14</f>
-        <v>41.542712391364333</v>
+        <f>Calculations!Y4</f>
+        <v>0</v>
       </c>
       <c r="X2" s="8">
-        <f>Calculations!Z3*About!$A$13*About!$A$14</f>
-        <v>41.127285267450688</v>
+        <f>Calculations!Z4</f>
+        <v>0</v>
       </c>
       <c r="Y2" s="8">
-        <f>Calculations!AA3*About!$A$13*About!$A$14</f>
-        <v>40.716012414776188</v>
+        <f>Calculations!AA4</f>
+        <v>0</v>
       </c>
       <c r="Z2" s="8">
-        <f>Calculations!AB3*About!$A$13*About!$A$14</f>
-        <v>40.308852290628423</v>
+        <f>Calculations!AB4</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="8">
-        <f>Calculations!AC3*About!$A$13*About!$A$14</f>
-        <v>39.905763767722142</v>
+        <f>Calculations!AC4</f>
+        <v>0</v>
       </c>
       <c r="AB2" s="8">
-        <f>Calculations!AD3*About!$A$13*About!$A$14</f>
-        <v>39.506706130044918</v>
+        <f>Calculations!AD4</f>
+        <v>0</v>
       </c>
       <c r="AC2" s="8">
-        <f>Calculations!AE3*About!$A$13*About!$A$14</f>
-        <v>39.111639068744466</v>
+        <f>Calculations!AE4</f>
+        <v>0</v>
       </c>
       <c r="AD2" s="8">
-        <f>Calculations!AF3*About!$A$13*About!$A$14</f>
-        <v>38.720522678057023</v>
+        <f>Calculations!AF4</f>
+        <v>0</v>
       </c>
       <c r="AE2" s="8">
-        <f>Calculations!AG3*About!$A$13*About!$A$14</f>
-        <v>38.33331745127645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B3"/>
+        <f>Calculations!AG4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="C3" s="7"/>
     </row>
   </sheetData>
@@ -1081,9 +1176,9 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1186,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1106,6 +1201,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -1334,27 +1449,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42629057-6501-4BCD-ADDE-2769C765847E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AF123D-D771-4054-8238-EEAACFB07BC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F07FEF0-D9CD-4745-AA90-3B402C6D0735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1371,23 +1485,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AF123D-D771-4054-8238-EEAACFB07BC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42629057-6501-4BCD-ADDE-2769C765847E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>